<commit_message>
Protege celdas antes valores incorrectos
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="973" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -121,13 +121,36 @@
     <t xml:space="preserve">xcvxcv</t>
   </si>
   <si>
-    <t xml:space="preserve">sdkfjklsdfjldksf
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sdkfjklsdfjldksf
 - sdlkfjlksdjfldksjflksjfdss
 - slkdjflksjflksjflksjkljfksldjfldks
 sldkjflskdjfdlskjflksdjflkdsjflkjslkfjslkjfdlskjflsjklfdjslkjlskjdflks
 klsdjfkljsdlkfjskldf
 sdklfjklsdjfklsdjflksdjfklsdjkl
-lñklllllllllllllllllllllllqweqweqweqew</t>
+Lñklllllllllllllllllllllllqweqweqweqew
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fgedfgdfgdffg
+Dfsfdf
+</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Difícil</t>
@@ -140,7 +163,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -165,6 +188,14 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -271,18 +302,18 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="54.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="53.4591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -428,85 +459,17 @@
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <dataValidations count="20">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D4" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D5" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D6" type="list">
-      <formula1>"Mínimo,Importante,Opcional"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E2" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E3" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E4" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E5" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E6" type="list">
-      <formula1>"Técnico,Funcional,Información"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F2" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F3" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F4" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F5" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F6" type="list">
-      <formula1>"Fácil,Media,Difícil"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G2" type="list">
+  <dataValidations count="3">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2:G6" type="list">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G3" type="list">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F6" type="list">
       <formula1>"v1,v2,v3"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G4" type="list">
-      <formula1>"v1,v2,v3"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G5" type="list">
-      <formula1>"v1,v2,v3"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="G6" type="list">
-      <formula1>"v1,v2,v3"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D1:E6" type="none">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Se añaden más requisitos
</commit_message>
<xml_diff>
--- a/requisitos.xlsx
+++ b/requisitos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="306">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -490,7 +490,7 @@
     <t xml:space="preserve">Eventos</t>
   </si>
   <si>
-    <t xml:space="preserve">Son los eventos deportivos que aparecerán en la aplicaciión. Se almacenará: Nombre, Deporte, Lugar, Organizador, participantes, resultados y realizado (sí o no).</t>
+    <t xml:space="preserve">Son los eventos deportivos que aparecerán en la aplicaciión. Se almacenará: Nombre, Deporte, Lugar, Organizador, participantes, pagina oficial, resultados y realizado (sí o no).</t>
   </si>
   <si>
     <t xml:space="preserve">R54</t>
@@ -542,6 +542,402 @@
   </si>
   <si>
     <t xml:space="preserve">Se mostrarán los resultados en un PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recuperar contraseña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un usuario puede cambiar su contraseña si no la recuerda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar eventos por nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se podrá buscar eventos por su nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar eventos por tipo de deporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se buscará eventos por el tipo de deporte que se indique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La web mostrará un chat general para todos los usuarios logueados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salas de chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada evento dispondrá de una sala de chat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valorar evento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se podrá valorar el evento con un sistema de votación que irá del 1 al 5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking de usuarios creadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking donde se mostrará los usuarios con más eventos creados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking de usuarios con más comentarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking donde se mostrará los usuarios con más comentarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking de usuarios con más votos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking donde se mostrará los usuarios con más votos a los eventos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recibir notificaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si el usuario lo desea, se mandará un correo cada vez que haya un nuevo evento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguir deporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se podrá seguir un deporte y recibir notificaciones de los eventos de ese deporte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deporte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se almacenará el nombre del deporte, descripción, si se juegan por equipos o de forma individual.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filtrar eventos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se filtrarán eventos por si se practican de forma individual o por equipos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar por fechas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscador para buscar eventos que se realizan desde una fecha hasta otra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar eventos del mes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En la página principal se mostrarán los eventos del mes actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Puntuación media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada evento muestra su puntuación media en base a las valoraciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Página oficial del evento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cada evento, si dispone de ella, mostrará un enlace a su página</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar participantes del torneo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando se ve los detalles de un evento, se mostrarán los participantes de este, de forma paginada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguir usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un usuario podrá seguir a otro y ver todo los eventos que realiza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfil de usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se mostrará una página de perfil de cada usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventos realizados por usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el perfil del usuario se podrá ver cada evento en el que se ha inscrito el usuario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventos creados por el usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el perfil del usuario se podrá ver cada evento que ha creado el usuario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Votar comentarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se podrán votar los comentarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comentar perfil de usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otros usuarios podrán comentar el perfil de otro usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartir por redes sociales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se podrán compartir un evento por redes sociales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subir cartel del evento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al crear  un evento se podrá subir un cartel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formulario de contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicación incluirá un formulario de contacto, que podrá usarse por los usuarios para realizar consultas, sugerencias o lo que deseen al administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Encuestas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el evento se podrá añadir, si el creador lo desea, encuestas para conocer la opinión de los usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promociones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para incentivar el pago a través de la aplicación, se mostrarán los eventos que dispongan de descuentos al pagar a través de la aplicación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preguntas frecuentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Página donde se mostrarán las preguntas frecuentes, acerca del uso de la aplicación, que pueden tener los usuarios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buscar por lugar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se mostrarán los eventos del lugar o ciudad que se indiquen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Videos de Youtube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En los detalles del evento, se podrán añadir videos de Youtube</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denunciar comentario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se podrán denunciar comentarios si son irrespetuosos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminación de comentarios con denuncias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicación tendrá la capacidad de eliminar comentarios que tengan un determinado número de denuncias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artículos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artículos informativos sobre eventos. Se almacenará, el contenido del artículo, id del usuario creador del artículo, id del evento al que se refiere.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear artículos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los usuarios logueados pueden crear artículos sobre los eventos que existen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificar artículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El creador del artículo podrá modificarlo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar artículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El creador del artículo podrá eliminarlo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denunciar artículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los usuarios podrán denunciar un artículo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminación de artículos con denuncias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicación tendrá la capacidad de eliminar artículos que tengan un determinado número de denuncias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validación de usuarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los usuarios recibirán un email para validar su cuenta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restricción del uso para usuarios no validados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los usuarios no validados no podrán acceder a la aplicación.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminación de usuarios no validados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasado un determinado tiempo, si el usuario no se ha validado, la aplicación borrará su cuenta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mapas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el evento se mostrará la ubicación de este mediante Google Maps</t>
   </si>
 </sst>
 </file>
@@ -683,21 +1079,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G61" activeCellId="0" sqref="G61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="51.5663265306123"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="50.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="4" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1717,7 +2113,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>132</v>
       </c>
@@ -2036,6 +2432,1018 @@
         <v>25</v>
       </c>
       <c r="G60" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G96" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G99" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G102" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" s="4" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>